<commit_message>
Subindo a finalização do MVP do bot para as agêncas do ES.
</commit_message>
<xml_diff>
--- a/app/data/depara_agencias.xlsx
+++ b/app/data/depara_agencias.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E713118\OneDrive - EDP\Documentos\automacao_suprimentos\app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E713118\OneDrive - EDP\Documentos\BOT-AGÊNCIAS\automacao_suprimentos\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>codigo_agencia</t>
   </si>
@@ -35,41 +35,450 @@
     <t>dono_area</t>
   </si>
   <si>
-    <t>tipo_agencia</t>
-  </si>
-  <si>
     <t>A001</t>
   </si>
   <si>
     <t>A002</t>
   </si>
   <si>
-    <t>Agência Centro</t>
-  </si>
-  <si>
-    <t>Agência Praia</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Independente</t>
-  </si>
-  <si>
-    <t>Erick</t>
-  </si>
-  <si>
-    <t>Joãozinho</t>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>Afonso Claudio</t>
+  </si>
+  <si>
+    <t>Agua Doce do Norte</t>
+  </si>
+  <si>
+    <t>Alegre</t>
+  </si>
+  <si>
+    <t>Alfredo Chaves</t>
+  </si>
+  <si>
+    <t>Anchieta</t>
+  </si>
+  <si>
+    <t>Apiaca</t>
+  </si>
+  <si>
+    <t>Aracruz</t>
+  </si>
+  <si>
+    <t>Atilio Vivacqua</t>
+  </si>
+  <si>
+    <t>Baixo Guandu</t>
+  </si>
+  <si>
+    <t>Barra de Sao Francisco</t>
+  </si>
+  <si>
+    <t>Boa Esperanca</t>
+  </si>
+  <si>
+    <t>Bom Jesus do Norte</t>
+  </si>
+  <si>
+    <t>Brejetuba</t>
+  </si>
+  <si>
+    <t>Cachoeiro de Itapemirim</t>
+  </si>
+  <si>
+    <t>Cariacica</t>
+  </si>
+  <si>
+    <t>Castelo</t>
+  </si>
+  <si>
+    <t>Conceicao da Barra</t>
+  </si>
+  <si>
+    <t>Conceicao do Castelo</t>
+  </si>
+  <si>
+    <t>Divino Sao Lourenco</t>
+  </si>
+  <si>
+    <t>Domingos Martins</t>
+  </si>
+  <si>
+    <t>Dores do Rio Preto</t>
+  </si>
+  <si>
+    <t>Ecoporanga</t>
+  </si>
+  <si>
+    <t>Fundao</t>
+  </si>
+  <si>
+    <t>Guacui</t>
+  </si>
+  <si>
+    <t>Guarapari</t>
+  </si>
+  <si>
+    <t>Ibatiba</t>
+  </si>
+  <si>
+    <t>Ibiracu</t>
+  </si>
+  <si>
+    <t>Ibitirama</t>
+  </si>
+  <si>
+    <t>Iconha</t>
+  </si>
+  <si>
+    <t>Irupi</t>
+  </si>
+  <si>
+    <t>Itaguacu</t>
+  </si>
+  <si>
+    <t>Itapemirim</t>
+  </si>
+  <si>
+    <t>Itarana</t>
+  </si>
+  <si>
+    <t>Iuna</t>
+  </si>
+  <si>
+    <t>Jaguare</t>
+  </si>
+  <si>
+    <t>Jeronimo Monteiro</t>
+  </si>
+  <si>
+    <t>Joao Neiva</t>
+  </si>
+  <si>
+    <t>Laranja da Terra</t>
+  </si>
+  <si>
+    <t>Linhares</t>
+  </si>
+  <si>
+    <t>Mantenopolis</t>
+  </si>
+  <si>
+    <t>Marataizes</t>
+  </si>
+  <si>
+    <t>Marechal Floriano</t>
+  </si>
+  <si>
+    <t>Mimoso do Sul</t>
+  </si>
+  <si>
+    <t>Montanha</t>
+  </si>
+  <si>
+    <t>Mucurici</t>
+  </si>
+  <si>
+    <t>Muniz Freire</t>
+  </si>
+  <si>
+    <t>Muqui</t>
+  </si>
+  <si>
+    <t>Nova Venecia</t>
+  </si>
+  <si>
+    <t>Pedro Canario</t>
+  </si>
+  <si>
+    <t>Pinheiros</t>
+  </si>
+  <si>
+    <t>Piuma</t>
+  </si>
+  <si>
+    <t>Ponto Belo</t>
+  </si>
+  <si>
+    <t>Presidente Kennedy</t>
+  </si>
+  <si>
+    <t>Rio Bananal</t>
+  </si>
+  <si>
+    <t>Rio Novo do Sul</t>
+  </si>
+  <si>
+    <t>Santa Leopoldina</t>
+  </si>
+  <si>
+    <t>Santa Maria de Jetiba</t>
+  </si>
+  <si>
+    <t>Santa Teresa</t>
+  </si>
+  <si>
+    <t>Sao Mateus</t>
+  </si>
+  <si>
+    <t>Serra</t>
+  </si>
+  <si>
+    <t>Sooretama</t>
+  </si>
+  <si>
+    <t>Vargem Alta</t>
+  </si>
+  <si>
+    <t>Venda Nova do Imigrante</t>
+  </si>
+  <si>
+    <t>Viana</t>
+  </si>
+  <si>
+    <t>Vila Pavao</t>
+  </si>
+  <si>
+    <t>Vila Valerio</t>
+  </si>
+  <si>
+    <t>Vila Velha</t>
+  </si>
+  <si>
+    <t>Vitoria</t>
+  </si>
+  <si>
+    <t>A004</t>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>A006</t>
+  </si>
+  <si>
+    <t>A007</t>
+  </si>
+  <si>
+    <t>A008</t>
+  </si>
+  <si>
+    <t>A009</t>
+  </si>
+  <si>
+    <t>A010</t>
+  </si>
+  <si>
+    <t>A011</t>
+  </si>
+  <si>
+    <t>A012</t>
+  </si>
+  <si>
+    <t>A013</t>
+  </si>
+  <si>
+    <t>A014</t>
+  </si>
+  <si>
+    <t>A015</t>
+  </si>
+  <si>
+    <t>A016</t>
+  </si>
+  <si>
+    <t>A017</t>
+  </si>
+  <si>
+    <t>A018</t>
+  </si>
+  <si>
+    <t>A019</t>
+  </si>
+  <si>
+    <t>A020</t>
+  </si>
+  <si>
+    <t>A021</t>
+  </si>
+  <si>
+    <t>A022</t>
+  </si>
+  <si>
+    <t>A023</t>
+  </si>
+  <si>
+    <t>A024</t>
+  </si>
+  <si>
+    <t>A025</t>
+  </si>
+  <si>
+    <t>A026</t>
+  </si>
+  <si>
+    <t>A027</t>
+  </si>
+  <si>
+    <t>A028</t>
+  </si>
+  <si>
+    <t>A029</t>
+  </si>
+  <si>
+    <t>A030</t>
+  </si>
+  <si>
+    <t>A031</t>
+  </si>
+  <si>
+    <t>A032</t>
+  </si>
+  <si>
+    <t>A033</t>
+  </si>
+  <si>
+    <t>A034</t>
+  </si>
+  <si>
+    <t>A035</t>
+  </si>
+  <si>
+    <t>A036</t>
+  </si>
+  <si>
+    <t>A037</t>
+  </si>
+  <si>
+    <t>A038</t>
+  </si>
+  <si>
+    <t>A039</t>
+  </si>
+  <si>
+    <t>A040</t>
+  </si>
+  <si>
+    <t>A041</t>
+  </si>
+  <si>
+    <t>A042</t>
+  </si>
+  <si>
+    <t>A043</t>
+  </si>
+  <si>
+    <t>A044</t>
+  </si>
+  <si>
+    <t>A045</t>
+  </si>
+  <si>
+    <t>A046</t>
+  </si>
+  <si>
+    <t>A047</t>
+  </si>
+  <si>
+    <t>A048</t>
+  </si>
+  <si>
+    <t>A049</t>
+  </si>
+  <si>
+    <t>A050</t>
+  </si>
+  <si>
+    <t>A051</t>
+  </si>
+  <si>
+    <t>A052</t>
+  </si>
+  <si>
+    <t>A053</t>
+  </si>
+  <si>
+    <t>A054</t>
+  </si>
+  <si>
+    <t>A055</t>
+  </si>
+  <si>
+    <t>A056</t>
+  </si>
+  <si>
+    <t>A057</t>
+  </si>
+  <si>
+    <t>A058</t>
+  </si>
+  <si>
+    <t>A059</t>
+  </si>
+  <si>
+    <t>A060</t>
+  </si>
+  <si>
+    <t>A061</t>
+  </si>
+  <si>
+    <t>A062</t>
+  </si>
+  <si>
+    <t>A063</t>
+  </si>
+  <si>
+    <t>A064</t>
+  </si>
+  <si>
+    <t>A065</t>
+  </si>
+  <si>
+    <t>A066</t>
+  </si>
+  <si>
+    <t>A067</t>
+  </si>
+  <si>
+    <t>A068</t>
+  </si>
+  <si>
+    <t>Sao Jose do Calcado</t>
+  </si>
+  <si>
+    <t>A069</t>
+  </si>
+  <si>
+    <t>email_responsavel</t>
+  </si>
+  <si>
+    <t>erickribgo200212@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,13 +501,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -115,13 +531,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D3" totalsRowShown="0">
-  <autoFilter ref="A1:D3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D70" totalsRowShown="0">
+  <autoFilter ref="A1:D70"/>
   <tableColumns count="4">
     <tableColumn id="1" name="codigo_agencia"/>
     <tableColumn id="2" name="nome_agencia"/>
-    <tableColumn id="3" name="tipo_agencia"/>
     <tableColumn id="4" name="dono_area"/>
+    <tableColumn id="3" name="email_responsavel"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -390,18 +806,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -412,59 +828,581 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
+      <c r="D2" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>129</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>135</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_activity xmlns="3e86c47f-7ef2-446d-8361-5b1e59315ed9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -473,7 +1411,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100524751B973301449AC7C4389EBDBF61D" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="37daa1cb7e7c63993a636ed6324543cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="3e86c47f-7ef2-446d-8361-5b1e59315ed9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="405bff7e879364195dfb16801c6960d1" ns1:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -640,24 +1578,17 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09A141A4-004D-4BC2-9FCF-445CF89D2886}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e86c47f-7ef2-446d-8361-5b1e59315ed9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="3e86c47f-7ef2-446d-8361-5b1e59315ed9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55081955-BAB4-4499-83B2-8F68DE0211B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -665,7 +1596,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53F5778-7610-4BB7-AFB3-F35BA251F6F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -682,4 +1613,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09A141A4-004D-4BC2-9FCF-445CF89D2886}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e86c47f-7ef2-446d-8361-5b1e59315ed9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>